<commit_message>
Committed as on 17/09/2019
</commit_message>
<xml_diff>
--- a/data/Input.xlsx
+++ b/data/Input.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="16335" windowHeight="6435"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16170" windowHeight="7005" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Login Scenarios" sheetId="1" r:id="rId1"/>
-    <sheet name="Forgot Password" sheetId="2" r:id="rId2"/>
+    <sheet name="Valid Login Scenario" sheetId="1" r:id="rId1"/>
+    <sheet name="Invalid Login Scenarios" sheetId="2" r:id="rId2"/>
+    <sheet name="Invalid Scenarios 2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>UserName</t>
   </si>
@@ -33,14 +33,38 @@
     <t>eTitle</t>
   </si>
   <si>
-    <t>my_tickets</t>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>adsd123</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>field can't be blank</t>
+  </si>
+  <si>
+    <t>Email doesn't exist OR invalid password!</t>
+  </si>
+  <si>
+    <t>fefcccsdcs</t>
+  </si>
+  <si>
+    <t>123@gmail.com</t>
+  </si>
+  <si>
+    <t>expectedmessage</t>
+  </si>
+  <si>
+    <t>abcdrgregg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -61,6 +85,12 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,12 +117,13 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -393,8 +424,8 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -421,7 +452,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
@@ -450,12 +481,114 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B14" s="5"/>
+      <c r="C14" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>